<commit_message>
Added errors to old samples
</commit_message>
<xml_diff>
--- a/Cowgill16/NW-GC.xlsx
+++ b/Cowgill16/NW-GC.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="23" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2AC52B31-CCA5-433F-B677-BA25E67A9A5B}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dyvas\git\dz-caucasus\Cowgill16\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B820F1-14B2-4AAD-B38F-7C02388ACCAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1380" yWindow="1410" windowWidth="16875" windowHeight="10432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>Zircon Sample Number</t>
   </si>
@@ -188,13 +193,22 @@
   </si>
   <si>
     <t xml:space="preserve">100311-2A-g74 </t>
+  </si>
+  <si>
+    <t>238 Error</t>
+  </si>
+  <si>
+    <t>206 Error</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -232,11 +246,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -551,21 +568,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C52"/>
+  <dimension ref="A1:E52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:C1"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2:E52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="1" max="1" width="24.86328125" customWidth="1"/>
+    <col min="2" max="2" width="22.59765625" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -575,8 +592,14 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -586,8 +609,14 @@
       <c r="C2" s="2">
         <v>595.1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" s="4">
+        <v>14.93594903635892</v>
+      </c>
+      <c r="E2" s="4">
+        <v>13.453995975064799</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -597,8 +626,14 @@
       <c r="C3" s="2">
         <v>295.8</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" s="4">
+        <v>8.7616469498884726</v>
+      </c>
+      <c r="E3" s="4">
+        <v>46.530318419628813</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -608,8 +643,14 @@
       <c r="C4" s="2">
         <v>1535.3</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" s="4">
+        <v>35.256641446030471</v>
+      </c>
+      <c r="E4" s="4">
+        <v>114.57384539555369</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -619,8 +660,14 @@
       <c r="C5" s="2">
         <v>1201.3</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5" s="4">
+        <v>19.07871864514766</v>
+      </c>
+      <c r="E5" s="4">
+        <v>27.522078968247683</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -630,8 +677,14 @@
       <c r="C6" s="2">
         <v>634.29999999999995</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6" s="4">
+        <v>8.507919439091836</v>
+      </c>
+      <c r="E6" s="4">
+        <v>14.528292216708678</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -641,8 +694,14 @@
       <c r="C7" s="2">
         <v>613.70000000000005</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7" s="4">
+        <v>64.566596060886781</v>
+      </c>
+      <c r="E7" s="4">
+        <v>14.252632289586586</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -652,8 +711,14 @@
       <c r="C8" s="2">
         <v>584.79999999999995</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="D8" s="4">
+        <v>46.3602693531368</v>
+      </c>
+      <c r="E8" s="4">
+        <v>7.0152132774614415</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -663,8 +728,14 @@
       <c r="C9" s="2">
         <v>1214.5999999999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="D9" s="4">
+        <v>12.360170176578663</v>
+      </c>
+      <c r="E9" s="4">
+        <v>82.715163702493783</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -674,8 +745,14 @@
       <c r="C10" s="2">
         <v>521.1</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="D10" s="4">
+        <v>27.607062422016924</v>
+      </c>
+      <c r="E10" s="4">
+        <v>55.366576166041085</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -685,8 +762,14 @@
       <c r="C11" s="2">
         <v>472.3</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="D11" s="4">
+        <v>17.42649938380265</v>
+      </c>
+      <c r="E11" s="4">
+        <v>31.026272499314189</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -696,8 +779,14 @@
       <c r="C12" s="2">
         <v>621.1</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="D12" s="4">
+        <v>21.841914054915435</v>
+      </c>
+      <c r="E12" s="4">
+        <v>20.125603533513697</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -707,8 +796,14 @@
       <c r="C13" s="2">
         <v>413.1</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="D13" s="4">
+        <v>18.080632324085485</v>
+      </c>
+      <c r="E13" s="4">
+        <v>27.9086763539147</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -718,8 +813,14 @@
       <c r="C14" s="2">
         <v>543</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="D14" s="4">
+        <v>32.411394431523206</v>
+      </c>
+      <c r="E14" s="4">
+        <v>75.924196086093957</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
@@ -729,8 +830,14 @@
       <c r="C15" s="2">
         <v>570.20000000000005</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="D15" s="4">
+        <v>32.842823744248165</v>
+      </c>
+      <c r="E15" s="4">
+        <v>24.933418371787582</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
@@ -740,8 +847,14 @@
       <c r="C16" s="2">
         <v>470.8</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="D16" s="4">
+        <v>20.260840965920721</v>
+      </c>
+      <c r="E16" s="4">
+        <v>56.709556182600267</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -751,8 +864,14 @@
       <c r="C17" s="2">
         <v>591.9</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="D17" s="4">
+        <v>28.980553759108375</v>
+      </c>
+      <c r="E17" s="4">
+        <v>33.429958154714825</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -762,8 +881,14 @@
       <c r="C18" s="2">
         <v>565.70000000000005</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="D18" s="4">
+        <v>26.084745924716628</v>
+      </c>
+      <c r="E18" s="4">
+        <v>29.497372244956807</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
@@ -773,8 +898,14 @@
       <c r="C19" s="2">
         <v>313.89999999999998</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="D19" s="4">
+        <v>11.63220256701905</v>
+      </c>
+      <c r="E19" s="4">
+        <v>18.408927718758662</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
@@ -784,8 +915,14 @@
       <c r="C20" s="2">
         <v>803.3</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
+      <c r="D20" s="4">
+        <v>16.514900753769382</v>
+      </c>
+      <c r="E20" s="4">
+        <v>10.302723349828057</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
@@ -795,8 +932,14 @@
       <c r="C21" s="2">
         <v>623</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
+      <c r="D21" s="4">
+        <v>25.583380572513988</v>
+      </c>
+      <c r="E21" s="4">
+        <v>38.820383719307472</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
@@ -806,8 +949,14 @@
       <c r="C22" s="2">
         <v>283.39999999999998</v>
       </c>
-    </row>
-    <row r="23" spans="1:3">
+      <c r="D22" s="4">
+        <v>17.570731115137193</v>
+      </c>
+      <c r="E22" s="4">
+        <v>119.98249413693733</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>24</v>
       </c>
@@ -817,8 +966,14 @@
       <c r="C23" s="2">
         <v>619.5</v>
       </c>
-    </row>
-    <row r="24" spans="1:3">
+      <c r="D23" s="4">
+        <v>22.417394168158523</v>
+      </c>
+      <c r="E23" s="4">
+        <v>21.455147619861634</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
@@ -828,8 +983,14 @@
       <c r="C24" s="2">
         <v>620.79999999999995</v>
       </c>
-    </row>
-    <row r="25" spans="1:3">
+      <c r="D24" s="4">
+        <v>44.583515531892715</v>
+      </c>
+      <c r="E24" s="4">
+        <v>27.556703665964562</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>26</v>
       </c>
@@ -839,8 +1000,14 @@
       <c r="C25" s="2">
         <v>496.3</v>
       </c>
-    </row>
-    <row r="26" spans="1:3">
+      <c r="D25" s="4">
+        <v>22.665061936716484</v>
+      </c>
+      <c r="E25" s="4">
+        <v>70.068729124722353</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>27</v>
       </c>
@@ -850,8 +1017,14 @@
       <c r="C26" s="2">
         <v>681.9</v>
       </c>
-    </row>
-    <row r="27" spans="1:3">
+      <c r="D26" s="4">
+        <v>27.113497635422959</v>
+      </c>
+      <c r="E26" s="4">
+        <v>26.45806848565519</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>28</v>
       </c>
@@ -861,8 +1034,14 @@
       <c r="C27" s="2">
         <v>562.29999999999995</v>
       </c>
-    </row>
-    <row r="28" spans="1:3">
+      <c r="D27" s="4">
+        <v>22.417885612442433</v>
+      </c>
+      <c r="E27" s="4">
+        <v>44.35433454014867</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>29</v>
       </c>
@@ -872,8 +1051,14 @@
       <c r="C28" s="2">
         <v>644.79999999999995</v>
       </c>
-    </row>
-    <row r="29" spans="1:3">
+      <c r="D28" s="4">
+        <v>18.465086725060587</v>
+      </c>
+      <c r="E28" s="4">
+        <v>28.902742376506978</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>30</v>
       </c>
@@ -883,8 +1068,14 @@
       <c r="C29" s="2">
         <v>315.2</v>
       </c>
-    </row>
-    <row r="30" spans="1:3">
+      <c r="D29" s="4">
+        <v>4.2097018326925308</v>
+      </c>
+      <c r="E29" s="4">
+        <v>21.111356594467338</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
         <v>31</v>
       </c>
@@ -894,8 +1085,14 @@
       <c r="C30" s="2">
         <v>827</v>
       </c>
-    </row>
-    <row r="31" spans="1:3">
+      <c r="D30" s="4">
+        <v>80.066495692962349</v>
+      </c>
+      <c r="E30" s="4">
+        <v>120.16852327267628</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
         <v>32</v>
       </c>
@@ -905,8 +1102,14 @@
       <c r="C31" s="2">
         <v>317.5</v>
       </c>
-    </row>
-    <row r="32" spans="1:3">
+      <c r="D31" s="4">
+        <v>9.6892162543084339</v>
+      </c>
+      <c r="E31" s="4">
+        <v>7.6355784972492415</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
         <v>33</v>
       </c>
@@ -916,8 +1119,14 @@
       <c r="C32" s="2">
         <v>580.9</v>
       </c>
-    </row>
-    <row r="33" spans="1:3">
+      <c r="D32" s="4">
+        <v>17.018187146023763</v>
+      </c>
+      <c r="E32" s="4">
+        <v>24.338915828040172</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
         <v>34</v>
       </c>
@@ -927,8 +1136,14 @@
       <c r="C33" s="2">
         <v>317.60000000000002</v>
       </c>
-    </row>
-    <row r="34" spans="1:3">
+      <c r="D33" s="4">
+        <v>10.337412312791486</v>
+      </c>
+      <c r="E33" s="4">
+        <v>22.510396531032171</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
         <v>35</v>
       </c>
@@ -938,8 +1153,14 @@
       <c r="C34" s="2">
         <v>574.70000000000005</v>
       </c>
-    </row>
-    <row r="35" spans="1:3">
+      <c r="D34" s="4">
+        <v>35.33818526693193</v>
+      </c>
+      <c r="E34" s="4">
+        <v>117.57962967278488</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
         <v>36</v>
       </c>
@@ -949,8 +1170,14 @@
       <c r="C35" s="2">
         <v>631.1</v>
       </c>
-    </row>
-    <row r="36" spans="1:3">
+      <c r="D35" s="4">
+        <v>6.5068846339024162</v>
+      </c>
+      <c r="E35" s="4">
+        <v>20.702287049642962</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
         <v>37</v>
       </c>
@@ -960,8 +1187,14 @@
       <c r="C36" s="2">
         <v>638.79999999999995</v>
       </c>
-    </row>
-    <row r="37" spans="1:3">
+      <c r="D36" s="4">
+        <v>20.083814556476511</v>
+      </c>
+      <c r="E36" s="4">
+        <v>32.419569782229985</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
         <v>38</v>
       </c>
@@ -971,8 +1204,14 @@
       <c r="C37" s="2">
         <v>424.3</v>
       </c>
-    </row>
-    <row r="38" spans="1:3">
+      <c r="D37" s="4">
+        <v>10.985369916239307</v>
+      </c>
+      <c r="E37" s="4">
+        <v>19.750013106831091</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
         <v>39</v>
       </c>
@@ -982,8 +1221,14 @@
       <c r="C38" s="2">
         <v>648.79999999999995</v>
       </c>
-    </row>
-    <row r="39" spans="1:3">
+      <c r="D38" s="4">
+        <v>7.7845920649667164</v>
+      </c>
+      <c r="E38" s="4">
+        <v>34.176050183839664</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
         <v>40</v>
       </c>
@@ -993,8 +1238,14 @@
       <c r="C39" s="2">
         <v>643.4</v>
       </c>
-    </row>
-    <row r="40" spans="1:3">
+      <c r="D39" s="4">
+        <v>36.668605889849459</v>
+      </c>
+      <c r="E39" s="4">
+        <v>21.743170929549422</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
         <v>41</v>
       </c>
@@ -1004,8 +1255,14 @@
       <c r="C40" s="2">
         <v>602.6</v>
       </c>
-    </row>
-    <row r="41" spans="1:3">
+      <c r="D40" s="4">
+        <v>17.332363383247582</v>
+      </c>
+      <c r="E40" s="4">
+        <v>19.35518065479863</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
         <v>42</v>
       </c>
@@ -1015,8 +1272,14 @@
       <c r="C41" s="2">
         <v>648.1</v>
       </c>
-    </row>
-    <row r="42" spans="1:3">
+      <c r="D41" s="4">
+        <v>27.602704659402661</v>
+      </c>
+      <c r="E41" s="4">
+        <v>130.50189932743143</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="s">
         <v>43</v>
       </c>
@@ -1026,8 +1289,14 @@
       <c r="C42" s="2">
         <v>328.4</v>
       </c>
-    </row>
-    <row r="43" spans="1:3">
+      <c r="D42" s="4">
+        <v>8.8956105132135974</v>
+      </c>
+      <c r="E42" s="4">
+        <v>31.093845484323424</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
         <v>44</v>
       </c>
@@ -1037,8 +1306,14 @@
       <c r="C43" s="2">
         <v>717.5</v>
       </c>
-    </row>
-    <row r="44" spans="1:3">
+      <c r="D43" s="4">
+        <v>320.66243775594569</v>
+      </c>
+      <c r="E43" s="4">
+        <v>81.769236345035154</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
         <v>45</v>
       </c>
@@ -1048,8 +1323,14 @@
       <c r="C44" s="2">
         <v>424</v>
       </c>
-    </row>
-    <row r="45" spans="1:3">
+      <c r="D44" s="4">
+        <v>64.794799461847617</v>
+      </c>
+      <c r="E44" s="4">
+        <v>175.88425218310482</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
         <v>46</v>
       </c>
@@ -1059,8 +1340,14 @@
       <c r="C45" s="2">
         <v>570.5</v>
       </c>
-    </row>
-    <row r="46" spans="1:3">
+      <c r="D45" s="4">
+        <v>32.615753544294876</v>
+      </c>
+      <c r="E45" s="4">
+        <v>35.881119645479203</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
         <v>47</v>
       </c>
@@ -1070,8 +1357,14 @@
       <c r="C46" s="2">
         <v>449.5</v>
       </c>
-    </row>
-    <row r="47" spans="1:3">
+      <c r="D46" s="4">
+        <v>37.157358898641093</v>
+      </c>
+      <c r="E46" s="4">
+        <v>56.846086489482218</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
         <v>48</v>
       </c>
@@ -1081,8 +1374,14 @@
       <c r="C47" s="2">
         <v>612.79999999999995</v>
       </c>
-    </row>
-    <row r="48" spans="1:3">
+      <c r="D47" s="4">
+        <v>40.674308787380824</v>
+      </c>
+      <c r="E47" s="4">
+        <v>20.957748179820612</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
         <v>49</v>
       </c>
@@ -1092,8 +1391,14 @@
       <c r="C48" s="2">
         <v>470.3</v>
       </c>
-    </row>
-    <row r="49" spans="1:3">
+      <c r="D48" s="4">
+        <v>39.093545558640983</v>
+      </c>
+      <c r="E48" s="4">
+        <v>13.939150526896981</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
         <v>50</v>
       </c>
@@ -1103,8 +1408,14 @@
       <c r="C49" s="2">
         <v>836.8</v>
       </c>
-    </row>
-    <row r="50" spans="1:3">
+      <c r="D49" s="4">
+        <v>33.905309849780281</v>
+      </c>
+      <c r="E49" s="4">
+        <v>32.214371413194215</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
         <v>51</v>
       </c>
@@ -1114,8 +1425,14 @@
       <c r="C50" s="2">
         <v>1192.2</v>
       </c>
-    </row>
-    <row r="51" spans="1:3">
+      <c r="D50" s="4">
+        <v>45.877930989128686</v>
+      </c>
+      <c r="E50" s="4">
+        <v>15.447111629789561</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
         <v>52</v>
       </c>
@@ -1125,8 +1442,14 @@
       <c r="C51" s="2">
         <v>556.29999999999995</v>
       </c>
-    </row>
-    <row r="52" spans="1:3">
+      <c r="D51" s="4">
+        <v>23.553140255949245</v>
+      </c>
+      <c r="E51" s="4">
+        <v>46.635935648666248</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="s">
         <v>53</v>
       </c>
@@ -1135,6 +1458,12 @@
       </c>
       <c r="C52" s="2">
         <v>664.3</v>
+      </c>
+      <c r="D52" s="4">
+        <v>45.013809856838691</v>
+      </c>
+      <c r="E52" s="4">
+        <v>9.4789595638183641</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Trexler sample, plotting of EEC and Africa
</commit_message>
<xml_diff>
--- a/Cowgill16/NW-GC.xlsx
+++ b/Cowgill16/NW-GC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dyvas\git\dz-caucasus\Cowgill16\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B820F1-14B2-4AAD-B38F-7C02388ACCAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B63F9D23-94A7-4C8E-8980-C8189003DD68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="1410" windowWidth="16875" windowHeight="10432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="1380" yWindow="1410" windowWidth="16875" windowHeight="10432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -572,7 +572,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2:E52"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Final modifications to figures for defense version
</commit_message>
<xml_diff>
--- a/Cowgill16/NW-GC.xlsx
+++ b/Cowgill16/NW-GC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dyvas\git\dz-caucasus\Cowgill16\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABEAD5A5-2F89-4D0F-89C5-FA3E664AA0CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67D8A3FF-0260-47D9-B65E-E56A1AE7D29B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28898" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>Zircon Sample Number</t>
   </si>
@@ -205,16 +205,32 @@
   </si>
   <si>
     <t>235 Error</t>
+  </si>
+  <si>
+    <t>75_ratio</t>
+  </si>
+  <si>
+    <t>75_1s</t>
+  </si>
+  <si>
+    <t>68_ratio</t>
+  </si>
+  <si>
+    <t>68_1s</t>
+  </si>
+  <si>
+    <t>rho</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -227,6 +243,12 @@
       <name val="Times New Roman"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
@@ -252,11 +274,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -573,11 +602,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G52"/>
+  <dimension ref="A1:L52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H2" sqref="H2:L52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -588,7 +617,7 @@
     <col min="6" max="6" width="11.53125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -610,8 +639,23 @@
       <c r="G1" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -633,8 +677,23 @@
       <c r="G2" s="3">
         <v>12.310716558970967</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H2" s="5">
+        <v>0.76527451798834567</v>
+      </c>
+      <c r="I2" s="3">
+        <v>2.7965793209640935</v>
+      </c>
+      <c r="J2" s="5">
+        <v>9.2867747120522481E-2</v>
+      </c>
+      <c r="K2" s="3">
+        <v>2.7265692942124073</v>
+      </c>
+      <c r="L2" s="6">
+        <v>0.97496583550236982</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -656,8 +715,23 @@
       <c r="G3" s="3">
         <v>9.5807618708649329</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H3" s="5">
+        <v>0.41055818699033647</v>
+      </c>
+      <c r="I3" s="3">
+        <v>3.2417053370332578</v>
+      </c>
+      <c r="J3" s="5">
+        <v>5.7002016169574524E-2</v>
+      </c>
+      <c r="K3" s="3">
+        <v>2.5203036889468353</v>
+      </c>
+      <c r="L3" s="6">
+        <v>0.77746230052277521</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -679,8 +753,23 @@
       <c r="G4" s="3">
         <v>51.837077035581842</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H4" s="5">
+        <v>3.2047422807781651</v>
+      </c>
+      <c r="I4" s="3">
+        <v>6.6923677441089895</v>
+      </c>
+      <c r="J4" s="5">
+        <v>0.24372778320285252</v>
+      </c>
+      <c r="K4" s="3">
+        <v>2.7908641748165293</v>
+      </c>
+      <c r="L4" s="6">
+        <v>0.41702193924911096</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -702,8 +791,23 @@
       <c r="G5" s="3">
         <v>15.641919628205983</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H5" s="5">
+        <v>2.3248996750041369</v>
+      </c>
+      <c r="I5" s="3">
+        <v>2.2029270486439123</v>
+      </c>
+      <c r="J5" s="5">
+        <v>0.21031642167419853</v>
+      </c>
+      <c r="K5" s="3">
+        <v>1.7031600900748274</v>
+      </c>
+      <c r="L5" s="6">
+        <v>0.7731350391849181</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -725,8 +829,23 @@
       <c r="G6" s="3">
         <v>7.2853962542836825</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H6" s="5">
+        <v>0.91669574039032575</v>
+      </c>
+      <c r="I6" s="3">
+        <v>1.5001814091031562</v>
+      </c>
+      <c r="J6" s="5">
+        <v>0.10924295078544824</v>
+      </c>
+      <c r="K6" s="3">
+        <v>1.3401029595471206</v>
+      </c>
+      <c r="L6" s="6">
+        <v>0.89329393859657658</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -748,8 +867,23 @@
       <c r="G7" s="3">
         <v>55.677343030944826</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H7" s="5">
+        <v>0.63816616529169423</v>
+      </c>
+      <c r="I7" s="3">
+        <v>14.061699153020012</v>
+      </c>
+      <c r="J7" s="5">
+        <v>7.6779176236858745E-2</v>
+      </c>
+      <c r="K7" s="3">
+        <v>14.046184325978944</v>
+      </c>
+      <c r="L7" s="6">
+        <v>0.99889666057620541</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -771,8 +905,23 @@
       <c r="G8" s="3">
         <v>36.534905186123524</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H8" s="5">
+        <v>0.80156850848867933</v>
+      </c>
+      <c r="I8" s="3">
+        <v>8.0835260874360984</v>
+      </c>
+      <c r="J8" s="5">
+        <v>9.7738189612434703E-2</v>
+      </c>
+      <c r="K8" s="3">
+        <v>8.0770866293527384</v>
+      </c>
+      <c r="L8" s="6">
+        <v>0.99920338500628225</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -794,8 +943,23 @@
       <c r="G9" s="3">
         <v>24.537477946403214</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H9" s="5">
+        <v>1.0210889211980738</v>
+      </c>
+      <c r="I9" s="3">
+        <v>4.7823057667851776</v>
+      </c>
+      <c r="J9" s="5">
+        <v>9.1743821777406462E-2</v>
+      </c>
+      <c r="K9" s="3">
+        <v>2.2816531650710896</v>
+      </c>
+      <c r="L9" s="6">
+        <v>0.47710315407224402</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -817,8 +981,23 @@
       <c r="G10" s="3">
         <v>24.795954806297004</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H10" s="5">
+        <v>0.65884213232431987</v>
+      </c>
+      <c r="I10" s="3">
+        <v>6.1473550892531872</v>
+      </c>
+      <c r="J10" s="5">
+        <v>8.2709873059665012E-2</v>
+      </c>
+      <c r="K10" s="3">
+        <v>5.6060127286643651</v>
+      </c>
+      <c r="L10" s="6">
+        <v>0.91193897981666994</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -840,8 +1019,23 @@
       <c r="G11" s="3">
         <v>14.95672630764517</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H11" s="5">
+        <v>0.68880963347291935</v>
+      </c>
+      <c r="I11" s="3">
+        <v>3.6112429922110634</v>
+      </c>
+      <c r="J11" s="5">
+        <v>8.8412017632889459E-2</v>
+      </c>
+      <c r="K11" s="3">
+        <v>3.3279203133303987</v>
+      </c>
+      <c r="L11" s="6">
+        <v>0.9215442772774497</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -863,8 +1057,23 @@
       <c r="G12" s="3">
         <v>17.826098083305283</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H12" s="5">
+        <v>0.82125146101242075</v>
+      </c>
+      <c r="I12" s="3">
+        <v>3.8929204000950222</v>
+      </c>
+      <c r="J12" s="5">
+        <v>9.8468190143759224E-2</v>
+      </c>
+      <c r="K12" s="3">
+        <v>3.7797437348777674</v>
+      </c>
+      <c r="L12" s="6">
+        <v>0.97092756758794951</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -886,8 +1095,23 @@
       <c r="G13" s="3">
         <v>15.843976549235009</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H13" s="5">
+        <v>0.51251790263228247</v>
+      </c>
+      <c r="I13" s="3">
+        <v>4.6045852501388964</v>
+      </c>
+      <c r="J13" s="5">
+        <v>6.755754205782899E-2</v>
+      </c>
+      <c r="K13" s="3">
+        <v>4.4321221718634689</v>
+      </c>
+      <c r="L13" s="6">
+        <v>0.96254536100287758</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -909,8 +1133,23 @@
       <c r="G14" s="3">
         <v>29.673899264670808</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H14" s="5">
+        <v>0.77751980911331775</v>
+      </c>
+      <c r="I14" s="3">
+        <v>6.6791943487143479</v>
+      </c>
+      <c r="J14" s="5">
+        <v>9.6639118588393219E-2</v>
+      </c>
+      <c r="K14" s="3">
+        <v>5.7054069196214128</v>
+      </c>
+      <c r="L14" s="6">
+        <v>0.85420585503993107</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
@@ -932,8 +1171,23 @@
       <c r="G15" s="3">
         <v>27.11940521681106</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H15" s="5">
+        <v>0.71960379952669662</v>
+      </c>
+      <c r="I15" s="3">
+        <v>6.3809001331228279</v>
+      </c>
+      <c r="J15" s="5">
+        <v>8.8333832907177473E-2</v>
+      </c>
+      <c r="K15" s="3">
+        <v>6.2770209974511841</v>
+      </c>
+      <c r="L15" s="6">
+        <v>0.98372030066221949</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
@@ -955,8 +1209,23 @@
       <c r="G16" s="3">
         <v>19.289985162140511</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H16" s="5">
+        <v>0.63663123436835478</v>
+      </c>
+      <c r="I16" s="3">
+        <v>4.8832913098963324</v>
+      </c>
+      <c r="J16" s="5">
+        <v>8.1771339333161025E-2</v>
+      </c>
+      <c r="K16" s="3">
+        <v>4.1578823065599009</v>
+      </c>
+      <c r="L16" s="6">
+        <v>0.8514508028905956</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -978,8 +1247,23 @@
       <c r="G17" s="3">
         <v>23.146882125253398</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H17" s="5">
+        <v>0.90124734181674671</v>
+      </c>
+      <c r="I17" s="3">
+        <v>4.8081941081487605</v>
+      </c>
+      <c r="J17" s="5">
+        <v>0.10952920976946816</v>
+      </c>
+      <c r="K17" s="3">
+        <v>4.554013714667728</v>
+      </c>
+      <c r="L17" s="6">
+        <v>0.94713599580968311</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -1001,8 +1285,23 @@
       <c r="G18" s="3">
         <v>21.395922848342366</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H18" s="5">
+        <v>0.78491426766287697</v>
+      </c>
+      <c r="I18" s="3">
+        <v>4.7910640659949868</v>
+      </c>
+      <c r="J18" s="5">
+        <v>9.6549924762292891E-2</v>
+      </c>
+      <c r="K18" s="3">
+        <v>4.5956030063042217</v>
+      </c>
+      <c r="L18" s="6">
+        <v>0.95920299603629433</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
@@ -1024,8 +1323,23 @@
       <c r="G19" s="3">
         <v>10.133146565409788</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H19" s="5">
+        <v>0.4356604587170978</v>
+      </c>
+      <c r="I19" s="3">
+        <v>3.2885435004120449</v>
+      </c>
+      <c r="J19" s="5">
+        <v>6.0010586879094156E-2</v>
+      </c>
+      <c r="K19" s="3">
+        <v>3.187319564025374</v>
+      </c>
+      <c r="L19" s="6">
+        <v>0.96921921927625765</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
@@ -1047,8 +1361,23 @@
       <c r="G20" s="3">
         <v>11.910234158475134</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H20" s="5">
+        <v>1.3478853920255416</v>
+      </c>
+      <c r="I20" s="3">
+        <v>2.0431224649250641</v>
+      </c>
+      <c r="J20" s="5">
+        <v>0.14833681273669463</v>
+      </c>
+      <c r="K20" s="3">
+        <v>1.9832486014988668</v>
+      </c>
+      <c r="L20" s="6">
+        <v>0.97069492188839834</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
@@ -1070,8 +1399,23 @@
       <c r="G21" s="3">
         <v>21.370758120050027</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H21" s="5">
+        <v>0.91314806036720575</v>
+      </c>
+      <c r="I21" s="3">
+        <v>4.4089307575749075</v>
+      </c>
+      <c r="J21" s="5">
+        <v>0.10938898082232573</v>
+      </c>
+      <c r="K21" s="3">
+        <v>4.024831633088187</v>
+      </c>
+      <c r="L21" s="6">
+        <v>0.91288157024766026</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
@@ -1093,8 +1437,23 @@
       <c r="G22" s="3">
         <v>20.574651861589473</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H22" s="5">
+        <v>0.34128091576722769</v>
+      </c>
+      <c r="I22" s="3">
+        <v>7.9625265532293268</v>
+      </c>
+      <c r="J22" s="5">
+        <v>4.7643225112066277E-2</v>
+      </c>
+      <c r="K22" s="3">
+        <v>5.9935317205655227</v>
+      </c>
+      <c r="L22" s="6">
+        <v>0.75271732916667677</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>24</v>
       </c>
@@ -1116,8 +1475,23 @@
       <c r="G23" s="3">
         <v>17.470165755873154</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H23" s="5">
+        <v>0.95804854281044804</v>
+      </c>
+      <c r="I23" s="3">
+        <v>3.5160917803068581</v>
+      </c>
+      <c r="J23" s="5">
+        <v>0.1149568591634374</v>
+      </c>
+      <c r="K23" s="3">
+        <v>3.3727825797442157</v>
+      </c>
+      <c r="L23" s="6">
+        <v>0.95924190563929612</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
@@ -1139,8 +1513,23 @@
       <c r="G24" s="3">
         <v>34.758251720067506</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H24" s="5">
+        <v>0.89630675072973942</v>
+      </c>
+      <c r="I24" s="3">
+        <v>7.2395295803134685</v>
+      </c>
+      <c r="J24" s="5">
+        <v>0.10748339961587697</v>
+      </c>
+      <c r="K24" s="3">
+        <v>7.1259867731078916</v>
+      </c>
+      <c r="L24" s="6">
+        <v>0.98431627277077005</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>26</v>
       </c>
@@ -1162,8 +1551,23 @@
       <c r="G25" s="3">
         <v>22.382817061378489</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H25" s="5">
+        <v>0.72990312284228998</v>
+      </c>
+      <c r="I25" s="3">
+        <v>5.2236137739202846</v>
+      </c>
+      <c r="J25" s="5">
+        <v>9.2672128231876913E-2</v>
+      </c>
+      <c r="K25" s="3">
+        <v>4.1455069125629418</v>
+      </c>
+      <c r="L25" s="6">
+        <v>0.7936090017336348</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>27</v>
       </c>
@@ -1185,8 +1589,23 @@
       <c r="G26" s="3">
         <v>22.727557800476518</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H26" s="5">
+        <v>0.82589361056696631</v>
+      </c>
+      <c r="I26" s="3">
+        <v>4.9476811354329175</v>
+      </c>
+      <c r="J26" s="5">
+        <v>9.6260277040030581E-2</v>
+      </c>
+      <c r="K26" s="3">
+        <v>4.7899540711373048</v>
+      </c>
+      <c r="L26" s="6">
+        <v>0.96812101265660633</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>28</v>
       </c>
@@ -1208,8 +1627,23 @@
       <c r="G27" s="3">
         <v>20.314740932419767</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H27" s="5">
+        <v>0.67658945885034172</v>
+      </c>
+      <c r="I27" s="3">
+        <v>4.957068732260181</v>
+      </c>
+      <c r="J27" s="5">
+        <v>8.3352080101853188E-2</v>
+      </c>
+      <c r="K27" s="3">
+        <v>4.5198900647157441</v>
+      </c>
+      <c r="L27" s="6">
+        <v>0.91180701919678564</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>29</v>
       </c>
@@ -1231,8 +1665,23 @@
       <c r="G28" s="3">
         <v>15.739382658843965</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H28" s="5">
+        <v>0.88521940655709697</v>
+      </c>
+      <c r="I28" s="3">
+        <v>3.3009122306113254</v>
+      </c>
+      <c r="J28" s="5">
+        <v>0.10498060874329451</v>
+      </c>
+      <c r="K28" s="3">
+        <v>3.0149320491619092</v>
+      </c>
+      <c r="L28" s="6">
+        <v>0.91336328824579094</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>30</v>
       </c>
@@ -1254,8 +1703,23 @@
       <c r="G29" s="3">
         <v>4.4870038134892525</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H29" s="5">
+        <v>0.37094027297627813</v>
+      </c>
+      <c r="I29" s="3">
+        <v>1.6331957768925842</v>
+      </c>
+      <c r="J29" s="5">
+        <v>5.1065089127299623E-2</v>
+      </c>
+      <c r="K29" s="3">
+        <v>1.3441216806780782</v>
+      </c>
+      <c r="L29" s="6">
+        <v>0.82300095291422093</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
         <v>31</v>
       </c>
@@ -1277,8 +1741,23 @@
       <c r="G30" s="3">
         <v>71.418195008570478</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H30" s="5">
+        <v>0.96015622083623298</v>
+      </c>
+      <c r="I30" s="3">
+        <v>14.335485038455582</v>
+      </c>
+      <c r="J30" s="5">
+        <v>0.10447653156943103</v>
+      </c>
+      <c r="K30" s="3">
+        <v>13.129495239717066</v>
+      </c>
+      <c r="L30" s="6">
+        <v>0.91587380576915278</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
         <v>32</v>
       </c>
@@ -1300,8 +1779,23 @@
       <c r="G31" s="3">
         <v>8.4323750553066077</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H31" s="5">
+        <v>0.39722369221186765</v>
+      </c>
+      <c r="I31" s="3">
+        <v>2.9210622863929236</v>
+      </c>
+      <c r="J31" s="5">
+        <v>5.4627508936333037E-2</v>
+      </c>
+      <c r="K31" s="3">
+        <v>2.9017354474253354</v>
+      </c>
+      <c r="L31" s="6">
+        <v>0.99338362654654178</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
         <v>33</v>
       </c>
@@ -1323,8 +1817,23 @@
       <c r="G32" s="3">
         <v>14.123564988483679</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H32" s="5">
+        <v>0.8443105155485604</v>
+      </c>
+      <c r="I32" s="3">
+        <v>3.038213286991402</v>
+      </c>
+      <c r="J32" s="5">
+        <v>0.10312867049285657</v>
+      </c>
+      <c r="K32" s="3">
+        <v>2.8238448647834042</v>
+      </c>
+      <c r="L32" s="6">
+        <v>0.92944260262245237</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
         <v>34</v>
       </c>
@@ -1346,8 +1855,23 @@
       <c r="G33" s="3">
         <v>9.369731083786462</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H33" s="5">
+        <v>0.40118825698657373</v>
+      </c>
+      <c r="I33" s="3">
+        <v>3.2227985942531805</v>
+      </c>
+      <c r="J33" s="5">
+        <v>5.5171045453604697E-2</v>
+      </c>
+      <c r="K33" s="3">
+        <v>3.0669374077832048</v>
+      </c>
+      <c r="L33" s="6">
+        <v>0.95163793767692972</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
         <v>35</v>
       </c>
@@ -1369,8 +1893,23 @@
       <c r="G34" s="3">
         <v>36.780806183995594</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H34" s="5">
+        <v>0.62138511067529001</v>
+      </c>
+      <c r="I34" s="3">
+        <v>9.4477148408475831</v>
+      </c>
+      <c r="J34" s="5">
+        <v>7.6117333576555021E-2</v>
+      </c>
+      <c r="K34" s="3">
+        <v>7.7499294330873152</v>
+      </c>
+      <c r="L34" s="6">
+        <v>0.82029671339996157</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
         <v>36</v>
       </c>
@@ -1392,8 +1931,23 @@
       <c r="G35" s="3">
         <v>6.7889505518358533</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H35" s="5">
+        <v>0.79859892219364959</v>
+      </c>
+      <c r="I35" s="3">
+        <v>1.5058158782951474</v>
+      </c>
+      <c r="J35" s="5">
+        <v>9.5312704649465105E-2</v>
+      </c>
+      <c r="K35" s="3">
+        <v>1.1599575218045088</v>
+      </c>
+      <c r="L35" s="6">
+        <v>0.77031829623007309</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
         <v>37</v>
       </c>
@@ -1415,8 +1969,23 @@
       <c r="G36" s="3">
         <v>16.958843517990829</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H36" s="5">
+        <v>0.93861839006953141</v>
+      </c>
+      <c r="I36" s="3">
+        <v>3.4492860443957865</v>
+      </c>
+      <c r="J36" s="5">
+        <v>0.11162221085816162</v>
+      </c>
+      <c r="K36" s="3">
+        <v>3.1026528615231617</v>
+      </c>
+      <c r="L36" s="6">
+        <v>0.89950581702673915</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
         <v>38</v>
       </c>
@@ -1438,8 +2007,23 @@
       <c r="G37" s="3">
         <v>9.8848993506820193</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H37" s="5">
+        <v>0.4876956890625978</v>
+      </c>
+      <c r="I37" s="3">
+        <v>2.9695716554539238</v>
+      </c>
+      <c r="J37" s="5">
+        <v>6.3963997650006571E-2</v>
+      </c>
+      <c r="K37" s="3">
+        <v>2.8345713534546415</v>
+      </c>
+      <c r="L37" s="6">
+        <v>0.95453879627678273</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
         <v>39</v>
       </c>
@@ -1461,8 +2045,23 @@
       <c r="G38" s="3">
         <v>9.7480514617358835</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H38" s="5">
+        <v>0.90121717395161027</v>
+      </c>
+      <c r="I38" s="3">
+        <v>2.0252415540120654</v>
+      </c>
+      <c r="J38" s="5">
+        <v>0.10667647089688102</v>
+      </c>
+      <c r="K38" s="3">
+        <v>1.2527646187653063</v>
+      </c>
+      <c r="L38" s="6">
+        <v>0.61857540710812542</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
         <v>40</v>
       </c>
@@ -1484,8 +2083,23 @@
       <c r="G39" s="3">
         <v>27.746119295504798</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H39" s="5">
+        <v>0.99634787850346984</v>
+      </c>
+      <c r="I39" s="3">
+        <v>5.4738070417759719</v>
+      </c>
+      <c r="J39" s="5">
+        <v>0.11823491186253592</v>
+      </c>
+      <c r="K39" s="3">
+        <v>5.3797094954534668</v>
+      </c>
+      <c r="L39" s="6">
+        <v>0.98280948787482725</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
         <v>41</v>
       </c>
@@ -1507,8 +2121,23 @@
       <c r="G40" s="3">
         <v>14.399634556873991</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H40" s="5">
+        <v>0.78759676632464237</v>
+      </c>
+      <c r="I40" s="3">
+        <v>3.2185338626477895</v>
+      </c>
+      <c r="J40" s="5">
+        <v>9.5244803433510633E-2</v>
+      </c>
+      <c r="K40" s="3">
+        <v>3.0917790149197537</v>
+      </c>
+      <c r="L40" s="6">
+        <v>0.96061720859952104</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
         <v>42</v>
       </c>
@@ -1530,8 +2159,23 @@
       <c r="G41" s="3">
         <v>35.81541175704939</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H41" s="5">
+        <v>0.85377378921379865</v>
+      </c>
+      <c r="I41" s="3">
+        <v>7.6555059295838088</v>
+      </c>
+      <c r="J41" s="5">
+        <v>0.10109317525163232</v>
+      </c>
+      <c r="K41" s="3">
+        <v>4.663725839709465</v>
+      </c>
+      <c r="L41" s="6">
+        <v>0.60919890633054574</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="s">
         <v>43</v>
       </c>
@@ -1553,8 +2197,23 @@
       <c r="G42" s="3">
         <v>8.6883332055874689</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H42" s="5">
+        <v>0.38761409421727905</v>
+      </c>
+      <c r="I42" s="3">
+        <v>3.0631276843632853</v>
+      </c>
+      <c r="J42" s="5">
+        <v>5.3051885590981181E-2</v>
+      </c>
+      <c r="K42" s="3">
+        <v>2.7390895058020659</v>
+      </c>
+      <c r="L42" s="6">
+        <v>0.89421329701162133</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
         <v>44</v>
       </c>
@@ -1576,8 +2235,23 @@
       <c r="G43" s="3">
         <v>247.23237036630033</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H43" s="5">
+        <v>1.0390949939845597</v>
+      </c>
+      <c r="I43" s="3">
+        <v>46.858880335558887</v>
+      </c>
+      <c r="J43" s="5">
+        <v>0.11910255983659601</v>
+      </c>
+      <c r="K43" s="3">
+        <v>46.700409278145671</v>
+      </c>
+      <c r="L43" s="6">
+        <v>0.996618121127129</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
         <v>45</v>
       </c>
@@ -1599,8 +2273,23 @@
       <c r="G44" s="3">
         <v>60.980251823732232</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H44" s="5">
+        <v>0.54245077534536557</v>
+      </c>
+      <c r="I44" s="3">
+        <v>17.056447701871754</v>
+      </c>
+      <c r="J44" s="5">
+        <v>7.1154302945492853E-2</v>
+      </c>
+      <c r="K44" s="3">
+        <v>15.130670989122038</v>
+      </c>
+      <c r="L44" s="6">
+        <v>0.8870939162473801</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
         <v>46</v>
       </c>
@@ -1622,8 +2311,23 @@
       <c r="G45" s="3">
         <v>25.577069279555303</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H45" s="5">
+        <v>0.91793508495243004</v>
+      </c>
+      <c r="I45" s="3">
+        <v>5.2620014262468668</v>
+      </c>
+      <c r="J45" s="5">
+        <v>0.11266273370801556</v>
+      </c>
+      <c r="K45" s="3">
+        <v>4.9967631382102988</v>
+      </c>
+      <c r="L45" s="6">
+        <v>0.94959364953541081</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
         <v>47</v>
       </c>
@@ -1645,8 +2349,23 @@
       <c r="G46" s="3">
         <v>31.33888252858344</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H46" s="5">
+        <v>0.65435185947556207</v>
+      </c>
+      <c r="I46" s="3">
+        <v>7.8006764955537538</v>
+      </c>
+      <c r="J46" s="5">
+        <v>8.4853871144436252E-2</v>
+      </c>
+      <c r="K46" s="3">
+        <v>7.3692180128858586</v>
+      </c>
+      <c r="L46" s="6">
+        <v>0.94468960699577542</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
         <v>48</v>
       </c>
@@ -1668,8 +2387,23 @@
       <c r="G47" s="3">
         <v>31.636535928182354</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H47" s="5">
+        <v>0.88176771263096998</v>
+      </c>
+      <c r="I47" s="3">
+        <v>6.6470712099169917</v>
+      </c>
+      <c r="J47" s="5">
+        <v>0.10613215741382725</v>
+      </c>
+      <c r="K47" s="3">
+        <v>6.5759157202144083</v>
+      </c>
+      <c r="L47" s="6">
+        <v>0.98929521176237367</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
         <v>49</v>
       </c>
@@ -1691,8 +2425,23 @@
       <c r="G48" s="3">
         <v>31.074142478192726</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H48" s="5">
+        <v>0.68452384501456198</v>
+      </c>
+      <c r="I48" s="3">
+        <v>7.528739517844623</v>
+      </c>
+      <c r="J48" s="5">
+        <v>8.7939658040233737E-2</v>
+      </c>
+      <c r="K48" s="3">
+        <v>7.5024233388205914</v>
+      </c>
+      <c r="L48" s="6">
+        <v>0.99650457039167617</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
         <v>50</v>
       </c>
@@ -1714,8 +2463,23 @@
       <c r="G49" s="3">
         <v>25.346123998145799</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H49" s="5">
+        <v>1.4049112358307341</v>
+      </c>
+      <c r="I49" s="3">
+        <v>4.2721020564818133</v>
+      </c>
+      <c r="J49" s="5">
+        <v>0.15214957661554399</v>
+      </c>
+      <c r="K49" s="3">
+        <v>3.9827552969753572</v>
+      </c>
+      <c r="L49" s="6">
+        <v>0.93227063499865437</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
         <v>51</v>
       </c>
@@ -1737,8 +2501,23 @@
       <c r="G50" s="3">
         <v>30.051312302384758</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H50" s="5">
+        <v>2.2403130966796274</v>
+      </c>
+      <c r="I50" s="3">
+        <v>4.2794209871571525</v>
+      </c>
+      <c r="J50" s="5">
+        <v>0.20359226264062852</v>
+      </c>
+      <c r="K50" s="3">
+        <v>4.2072314512957609</v>
+      </c>
+      <c r="L50" s="6">
+        <v>0.98313100391897912</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
         <v>52</v>
       </c>
@@ -1760,8 +2539,23 @@
       <c r="G51" s="3">
         <v>20.910774751807025</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H51" s="5">
+        <v>0.75519182985722411</v>
+      </c>
+      <c r="I51" s="3">
+        <v>4.7857072499865145</v>
+      </c>
+      <c r="J51" s="5">
+        <v>9.329568160336664E-2</v>
+      </c>
+      <c r="K51" s="3">
+        <v>4.281586979132328</v>
+      </c>
+      <c r="L51" s="6">
+        <v>0.8946612810769804</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="s">
         <v>53</v>
       </c>
@@ -1782,6 +2576,21 @@
       </c>
       <c r="G52" s="3">
         <v>34.796873233326892</v>
+      </c>
+      <c r="H52" s="5">
+        <v>0.92718350729814303</v>
+      </c>
+      <c r="I52" s="3">
+        <v>7.1202905493921422</v>
+      </c>
+      <c r="J52" s="5">
+        <v>0.10896228452037698</v>
+      </c>
+      <c r="K52" s="3">
+        <v>7.1065871146249799</v>
+      </c>
+      <c r="L52" s="6">
+        <v>0.99807543882203908</v>
       </c>
     </row>
   </sheetData>

</xml_diff>